<commit_message>
Upload validation checks for all of the controlled vocabularies work
Next step is to make sure the free form ones don’t have any scripting
or any illegal characters etc.
</commit_message>
<xml_diff>
--- a/assets/uploads/upload_template_edited.xlsx
+++ b/assets/uploads/upload_template_edited.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="325">
   <si>
     <t>Female</t>
   </si>
@@ -1238,9 +1238,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1304,17 +1308,351 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="79">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1395,8 +1733,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="12"/>
-      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="wholeTable" dxfId="78"/>
+      <tableStyleElement type="headerRow" dxfId="77"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1672,7 +2010,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Integral" id="{3577F8C9-A904-41D8-97D2-FD898F53F20E}" vid="{682D6EBE-8D36-4FF2-9DB3-F3D8D7B6715D}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Integral" id="{3577F8C9-A904-41D8-97D2-FD898F53F20E}" vid="{682D6EBE-8D36-4FF2-9DB3-F3D8D7B6715D}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1684,7 +2022,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1860,88 +2198,214 @@
       </c>
       <c r="Z2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="14">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+    <row r="3" spans="1:26">
+      <c r="A3" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="H3" s="7">
+        <v>43018</v>
+      </c>
+      <c r="I3" s="5">
+        <v>44</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="5">
+        <v>22</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>324</v>
+      </c>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
+      <c r="V3" s="7">
+        <v>40461</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="X3" s="5">
+        <v>214</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>321</v>
+      </c>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" ht="14">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+    <row r="4" spans="1:26">
+      <c r="A4" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="H4" s="7">
+        <v>43018</v>
+      </c>
+      <c r="I4" s="5">
+        <v>44</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="5">
+        <v>22</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>324</v>
+      </c>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
+      <c r="V4" s="7">
+        <v>40461</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="X4" s="5">
+        <v>214</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>321</v>
+      </c>
       <c r="Z4" s="5"/>
     </row>
-    <row r="5" spans="1:26" ht="14">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
+    <row r="5" spans="1:26">
+      <c r="A5" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="H5" s="7">
+        <v>43018</v>
+      </c>
+      <c r="I5" s="5">
+        <v>44</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="5">
+        <v>22</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>324</v>
+      </c>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
+      <c r="V5" s="7">
+        <v>40461</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="X5" s="5">
+        <v>214</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>321</v>
+      </c>
       <c r="Z5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="14">
@@ -11381,19 +11845,64 @@
       <c r="Z342" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I301">
-    <cfRule type="expression" dxfId="10" priority="3">
+  <conditionalFormatting sqref="I2 I6:I301">
+    <cfRule type="expression" dxfId="76" priority="36">
       <formula>NOT(ISNUMBER(I2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q301">
-    <cfRule type="expression" dxfId="9" priority="2">
+  <conditionalFormatting sqref="Q2 Q6:Q301">
+    <cfRule type="expression" dxfId="75" priority="35">
       <formula>NOT(ISNUMBER(Q2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R301">
-    <cfRule type="expression" dxfId="8" priority="1">
+  <conditionalFormatting sqref="R2 R6:R301">
+    <cfRule type="expression" dxfId="74" priority="34">
       <formula>NOT(ISNUMBER(R2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="expression" dxfId="65" priority="25">
+      <formula>NOT(ISNUMBER(I3))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3">
+    <cfRule type="expression" dxfId="63" priority="24">
+      <formula>NOT(ISNUMBER(Q3))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3">
+    <cfRule type="expression" dxfId="61" priority="23">
+      <formula>NOT(ISNUMBER(R3))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4">
+    <cfRule type="expression" dxfId="43" priority="14">
+      <formula>NOT(ISNUMBER(I4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4">
+    <cfRule type="expression" dxfId="41" priority="13">
+      <formula>NOT(ISNUMBER(Q4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4">
+    <cfRule type="expression" dxfId="39" priority="12">
+      <formula>NOT(ISNUMBER(R4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="expression" dxfId="21" priority="3">
+      <formula>NOT(ISNUMBER(I5))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q5">
+    <cfRule type="expression" dxfId="19" priority="2">
+      <formula>NOT(ISNUMBER(Q5))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5">
+    <cfRule type="expression" dxfId="17" priority="1">
+      <formula>NOT(ISNUMBER(R5))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11402,7 +11911,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="19" id="{460C5720-7DC9-44F2-A583-2FB7F903B0CB}">
+          <x14:cfRule type="expression" priority="52" id="{460C5720-7DC9-44F2-A583-2FB7F903B0CB}">
             <xm:f>NOT(OR(E2=Lists!$A$2:$A$4))</xm:f>
             <x14:dxf>
               <font>
@@ -11410,10 +11919,10 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E2:E301</xm:sqref>
+          <xm:sqref>E2 E6:E301</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="18" id="{F603EC46-06FA-45DA-94F6-178D8094EE54}">
+          <x14:cfRule type="expression" priority="51" id="{F603EC46-06FA-45DA-94F6-178D8094EE54}">
             <xm:f>NOT(OR(F2=Lists!$B$2:$B$9))</xm:f>
             <x14:dxf>
               <font>
@@ -11421,10 +11930,10 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F2:F301</xm:sqref>
+          <xm:sqref>F2 F6:F301</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="16" id="{67A85774-3CCA-47AA-8D60-1BE7C594B919}">
+          <x14:cfRule type="expression" priority="49" id="{67A85774-3CCA-47AA-8D60-1BE7C594B919}">
             <xm:f>NOT(OR(G2=Lists!$C$2:$C$252))</xm:f>
             <x14:dxf>
               <font>
@@ -11432,10 +11941,10 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>G2:G301</xm:sqref>
+          <xm:sqref>G2 G6:G301</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="11" id="{5EC26868-599A-4E52-B449-E5E6C3964683}">
+          <x14:cfRule type="expression" priority="44" id="{5EC26868-599A-4E52-B449-E5E6C3964683}">
             <xm:f>NOT(OR(J2=Lists!$D$2:$D$4))</xm:f>
             <x14:dxf>
               <font>
@@ -11443,10 +11952,10 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>J2:J301</xm:sqref>
+          <xm:sqref>J2 J6:J301</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="9" id="{4194D672-3B74-42BC-8E9A-F2D44455AB4A}">
+          <x14:cfRule type="expression" priority="42" id="{4194D672-3B74-42BC-8E9A-F2D44455AB4A}">
             <xm:f>NOT(OR(K2=Lists!$E$2:$E$6))</xm:f>
             <x14:dxf>
               <font>
@@ -11454,10 +11963,10 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>K2:K301</xm:sqref>
+          <xm:sqref>K2 K6:K301</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="7" id="{70CE586C-B690-4795-ABF9-ED6AA9D358A1}">
+          <x14:cfRule type="expression" priority="40" id="{70CE586C-B690-4795-ABF9-ED6AA9D358A1}">
             <xm:f>NOT(OR(M2=Lists!$F$2:$F$9))</xm:f>
             <x14:dxf>
               <font>
@@ -11465,10 +11974,10 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>M2:M301</xm:sqref>
+          <xm:sqref>M2 M6:M301</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="6" id="{1A817AE9-7F2B-48A2-B26A-616154B760FB}">
+          <x14:cfRule type="expression" priority="39" id="{1A817AE9-7F2B-48A2-B26A-616154B760FB}">
             <xm:f>NOT(OR(N2 = Lists!$G$2:$G$6))</xm:f>
             <x14:dxf>
               <font>
@@ -11476,10 +11985,10 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>N2:N301</xm:sqref>
+          <xm:sqref>N2 N6:N301</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="5" id="{05BBB06D-3AA4-47A2-B19E-82C528A5F065}">
+          <x14:cfRule type="expression" priority="38" id="{05BBB06D-3AA4-47A2-B19E-82C528A5F065}">
             <xm:f>NOT(OR(V2=Lists!$H$2:$H$3))</xm:f>
             <x14:dxf>
               <font>
@@ -11487,7 +11996,271 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>V2:V301</xm:sqref>
+          <xm:sqref>V2 V6:V301</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="33" id="{8EDA9146-1B50-B442-804B-4E6455BF34F1}">
+            <xm:f>NOT(OR(E3=Lists!$A$2:$A$4))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="32" id="{C85049E3-7829-C94C-8B4C-74E0034AD462}">
+            <xm:f>NOT(OR(F3=Lists!$B$2:$B$9))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="31" id="{3A281FDC-296C-6C44-B506-743C34F72C30}">
+            <xm:f>NOT(OR(G3=Lists!$C$2:$C$252))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="30" id="{EF635E42-747C-3A4E-A43E-22066BFFC771}">
+            <xm:f>NOT(OR(J3=Lists!$D$2:$D$4))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="29" id="{D99E199C-2E2A-E441-940F-57BCB0309ADB}">
+            <xm:f>NOT(OR(K3=Lists!$E$2:$E$6))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>K3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="28" id="{2034292F-ECAC-2941-8A16-1A40E0B145B3}">
+            <xm:f>NOT(OR(M3=Lists!$F$2:$F$9))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>M3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="27" id="{7F434E45-F4D5-9E4B-930A-95E98EAED8E0}">
+            <xm:f>NOT(OR(N3 = Lists!$G$2:$G$6))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="26" id="{F4F5C8D0-1D71-5746-A3E5-AB91C80EE1A3}">
+            <xm:f>NOT(OR(V3=Lists!$H$2:$H$3))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>V3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="22" id="{089B9F00-83E2-4B45-9D4B-5D343851BCEA}">
+            <xm:f>NOT(OR(E4=Lists!$A$2:$A$4))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="21" id="{91108D39-AD00-7941-A709-D34D32EE78F5}">
+            <xm:f>NOT(OR(F4=Lists!$B$2:$B$9))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="20" id="{50219512-7591-6B4C-8EDC-B5494FC699F1}">
+            <xm:f>NOT(OR(G4=Lists!$C$2:$C$252))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="19" id="{5E57E814-C1C1-5D43-85E5-18B693CA5CDC}">
+            <xm:f>NOT(OR(J4=Lists!$D$2:$D$4))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="18" id="{85013141-045D-BC4F-8E9B-918FD22BD947}">
+            <xm:f>NOT(OR(K4=Lists!$E$2:$E$6))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>K4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="17" id="{516CD615-48A6-4842-9BC9-7876DF4A49E4}">
+            <xm:f>NOT(OR(M4=Lists!$F$2:$F$9))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>M4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="16" id="{630F0FB8-5833-8743-BE8A-8CEAF2D230F7}">
+            <xm:f>NOT(OR(N4 = Lists!$G$2:$G$6))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="15" id="{9B3F45AE-D232-8046-8FC6-EB21E15AE482}">
+            <xm:f>NOT(OR(V4=Lists!$H$2:$H$3))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>V4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="11" id="{D641D789-F077-1747-A178-6DE1D0FED857}">
+            <xm:f>NOT(OR(E5=Lists!$A$2:$A$4))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="10" id="{C6DB175F-FD85-2742-98B7-FB8EB62FEC83}">
+            <xm:f>NOT(OR(F5=Lists!$B$2:$B$9))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="9" id="{C3F9AA8A-EA03-A546-904B-513E8D3B7DFE}">
+            <xm:f>NOT(OR(G5=Lists!$C$2:$C$252))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="8" id="{D176E759-D4A6-B14F-8B29-7F42DD34C6DB}">
+            <xm:f>NOT(OR(J5=Lists!$D$2:$D$4))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>J5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="7" id="{AAEA102C-2A9F-C049-9C82-A6E34AF5553C}">
+            <xm:f>NOT(OR(K5=Lists!$E$2:$E$6))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>K5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="6" id="{EABF6E69-9EB7-D443-BFC3-F97BAA841B72}">
+            <xm:f>NOT(OR(M5=Lists!$F$2:$F$9))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>M5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="5" id="{1A1E8663-F60F-284E-B3E8-D2170DC10851}">
+            <xm:f>NOT(OR(N5 = Lists!$G$2:$G$6))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>N5</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="4" id="{F51775A5-AFE2-FE47-A80B-206C0258D14B}">
+            <xm:f>NOT(OR(V5=Lists!$H$2:$H$3))</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FFFF0000"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>V5</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>